<commit_message>
Update of Code and Readme.md
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhij\OneDrive\Desktop\Certificate database\web\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B94737-3251-4C7D-85E1-D298E44E30B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048E3C12-AD79-40F6-A95E-1746838B864F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>Scholar</t>
   </si>
   <si>
-    <t>https://drive.google.com/file/d/1-sYKOm7zmFrUHhtYOMA9rTx9svWzNMU6/view?usp=drive_link</t>
-  </si>
-  <si>
     <t>https://mega.nz/file/rB03DQZY#1UgMEcJAb4QbaGoZ6A-yEGqiqC100LoeeSwsQgzihHU</t>
   </si>
   <si>
@@ -412,13 +409,16 @@
   </si>
   <si>
     <t>https://mega.nz/file/DQlk3IxD#Mybds34hETPiJ1J0Um7IY8fAL8su41GXGNvD89d5TEk</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1POOBmBqGIMqNGuME0VsWmDRKv9yrRVez/view?usp=sharing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -441,19 +441,7 @@
     <font>
       <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
       <color rgb="FF434343"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
     <font>
@@ -483,14 +471,15 @@
     <font>
       <u/>
       <sz val="10"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF434343"/>
       <name val="Roboto"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
-      <color rgb="FF434343"/>
-      <name val="Roboto"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -690,10 +679,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -716,10 +706,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -728,29 +715,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
@@ -1073,7 +1058,9 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1125,42 +1112,42 @@
       <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="9" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="C3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>9</v>
@@ -1171,675 +1158,649 @@
       <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="14" t="s">
+      <c r="F4" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="B5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="F5" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>23</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="14" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="B7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="C7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="11" t="s">
+      <c r="E7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>31</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="14" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="B9" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="C9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="E9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="14" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="B11" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="C11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="F11" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="14" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="B13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="C13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="11" t="s">
+      <c r="E13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="14" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="B15" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="C15" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="11" t="s">
+      <c r="E15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G15" s="13" t="s">
         <v>64</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="14" t="s">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="B17" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="C17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="11" t="s">
+      <c r="E17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" s="14" t="s">
         <v>72</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="16" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="C18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="E18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="14" t="s">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="11" t="s">
+      <c r="E19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19" s="14" t="s">
         <v>80</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="16" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="7" t="s">
+      <c r="E20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="14" t="s">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="B21" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="C21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="F21" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" s="14" t="s">
         <v>89</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="E22" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="14" t="s">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="B23" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="11" t="s">
+      <c r="E23" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G23" s="14" t="s">
         <v>97</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="16" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="C24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="7" t="s">
+      <c r="E24" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="14" t="s">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="B25" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="C25" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="11" t="s">
+      <c r="E25" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G25" s="14" t="s">
         <v>105</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="C26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="7" t="s">
+      <c r="E26" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G26" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="14" t="s">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="B27" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="C27" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="11" t="s">
+      <c r="E27" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>113</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="C28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="7" t="s">
+      <c r="E28" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G28" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G28" s="14" t="s">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="B29" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="C29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="11" t="s">
+      <c r="E29" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G29" s="16" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="G30" s="15" t="s">
         <v>125</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="18" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="G2" r:id="rId2" location="1UgMEcJAb4QbaGoZ6A-yEGqiqC100LoeeSwsQgzihHU" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="G3" r:id="rId4" location="teyeaVagow-wpzrmJhiW3IMIUDgt5MbDuSuxVrg-258" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="G4" r:id="rId6" location="JFmU88vh7zjvNYDy0QIgFgNPZFSa3O8lxL_LSJ-_1Ps" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="F5" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="G5" r:id="rId8" location="we_NNyKrvU2kYT-5diQVtlxJF4o-gB_Qn-llJ7260jk" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="F6" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="G6" r:id="rId10" location="pMFVpEOSVQZYBCS7B5TmW6_PZ72SDF2gbG9vX2S1HAk" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="F7" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="G7" r:id="rId12" location="tWaXUmLOr6t9mJtl3fVA47vajR6_ZK9v7jtalFl6y64" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="F8" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="G8" r:id="rId14" location="GTspz0sBRcbbXjV7n2UtaqhPZ6N1kBYUWkTOigtRpvM" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="F9" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="G9" r:id="rId16" location="7Y5NbVNwfKCxiXTncwSAVXVDYGoF2uOl42jzT7an_Oo" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="F10" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="G10" r:id="rId18" location="1HglUBUhP72JBrjpEEgHGJEKHdHNWAxHz38JS9I57vQ" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="F11" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="G11" r:id="rId20" location="feM4zNWGEwI9taAYZ8a8qmk2v-vO0_lqo-1B7GMR86k" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="F12" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="G12" r:id="rId22" location="C-8GQya5aIfI1CsrkL1fSUolQf6FBXq2XJaBTILKIlA" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="F13" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="G13" r:id="rId24" location="bAvQOAOfIsuurMmkTQWOd7DPraIDkxNzSBo4Jzckv24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="F14" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="G14" r:id="rId26" location="wi59MsAL_ZXfpz803yJwUJzHAFc2aybh_yOk9f8eV4A" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="F15" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="G15" r:id="rId28" location="AGqWP6aBZCidiqzF9J_6NbUC0E8pEmZ-ZetlwZtZ1KI" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="F16" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="G16" r:id="rId30" location="9WO-4DyyvXQwLlHaRf5NUVu2pcS_UbGMkj2D4_UKdSQ" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="F17" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="G17" r:id="rId32" location="j2yeVLpqgoWyqqqHOnewN60Dk-V6cRRyu87lDMcAWII" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="F18" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="G18" r:id="rId34" location="AEbLyKurqObK-gYoAC8AaE5ltStqotESAc5gctJTiHs" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="F19" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="G19" r:id="rId36" location="0HMjhkh35Fr7DZToaFH2mmITpO4Rul2mM81aUdwOoVM" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="F20" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="G20" r:id="rId38" location="VFJC_ZJU0jj8yBDFlxVpdt6LxmTO-ZySo9V1dpcMfh8" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="F21" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="G21" r:id="rId40" location="Nfi_lJ9ZpKk9RhLwSOvYd5mRaPkKkM4B-4cqv4ppf9U" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="F22" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="G22" r:id="rId42" location="J7fEN89thcXGn94n15_wJl74cQGBn-RLoTnk3k_IA-M" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="F23" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="G23" r:id="rId44" location="RZdhhHAXIkrJU1UReZqf2Eh1govJXu56xGzk0ykyTo0" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="F24" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="G24" r:id="rId46" location="W7S5VFDoc2APi-3aQywqFBSyXAkUHKzWukN-60mtIks" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="F25" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="G25" r:id="rId48" location="jIRKBORNkHhaBRHyCepl14wBYWbNUyitK7j2mLENKbc" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="F26" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="G26" r:id="rId50" location="SfZujTtD9DXzAflWaw8q5a4mcrX8-k37lIrTECb1gNs" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="F27" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="G27" r:id="rId52" location="X6KHI1GKOdaR5uSjSH6vUKkR4i0OP8ERWQqIaIf2U3Q" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="F28" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="G28" r:id="rId54" location="IR0hxJeFqvw3fVWLPeL9PTPx_Sk3ZRxeP9Bf2Vsr8Mc" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="F29" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
-    <hyperlink ref="G29" r:id="rId56" location="XunseXF_808g4CzMs1Ad2pXfI7krE2q0sTy6EET0nRA" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
-    <hyperlink ref="F30" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
-    <hyperlink ref="G30" r:id="rId58" location="rBDf6zRJ4qXP3i82sRKnLA6Hs9G_Gp9cDRIE7ZfkifA" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="G3" r:id="rId3" location="teyeaVagow-wpzrmJhiW3IMIUDgt5MbDuSuxVrg-258" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="G4" r:id="rId4" location="JFmU88vh7zjvNYDy0QIgFgNPZFSa3O8lxL_LSJ-_1Ps" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="G5" r:id="rId5" location="we_NNyKrvU2kYT-5diQVtlxJF4o-gB_Qn-llJ7260jk" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="G6" r:id="rId6" location="pMFVpEOSVQZYBCS7B5TmW6_PZ72SDF2gbG9vX2S1HAk" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="G7" r:id="rId7" location="tWaXUmLOr6t9mJtl3fVA47vajR6_ZK9v7jtalFl6y64" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="G8" r:id="rId8" location="GTspz0sBRcbbXjV7n2UtaqhPZ6N1kBYUWkTOigtRpvM" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="G9" r:id="rId9" location="7Y5NbVNwfKCxiXTncwSAVXVDYGoF2uOl42jzT7an_Oo" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="G10" r:id="rId10" location="1HglUBUhP72JBrjpEEgHGJEKHdHNWAxHz38JS9I57vQ" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="G11" r:id="rId11" location="feM4zNWGEwI9taAYZ8a8qmk2v-vO0_lqo-1B7GMR86k" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="G12" r:id="rId12" location="C-8GQya5aIfI1CsrkL1fSUolQf6FBXq2XJaBTILKIlA" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="G13" r:id="rId13" location="bAvQOAOfIsuurMmkTQWOd7DPraIDkxNzSBo4Jzckv24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="G14" r:id="rId14" location="wi59MsAL_ZXfpz803yJwUJzHAFc2aybh_yOk9f8eV4A" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="G15" r:id="rId15" location="AGqWP6aBZCidiqzF9J_6NbUC0E8pEmZ-ZetlwZtZ1KI" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="G16" r:id="rId16" location="9WO-4DyyvXQwLlHaRf5NUVu2pcS_UbGMkj2D4_UKdSQ" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="G17" r:id="rId17" location="j2yeVLpqgoWyqqqHOnewN60Dk-V6cRRyu87lDMcAWII" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="G18" r:id="rId18" location="AEbLyKurqObK-gYoAC8AaE5ltStqotESAc5gctJTiHs" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="G19" r:id="rId19" location="0HMjhkh35Fr7DZToaFH2mmITpO4Rul2mM81aUdwOoVM" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="G20" r:id="rId20" location="VFJC_ZJU0jj8yBDFlxVpdt6LxmTO-ZySo9V1dpcMfh8" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="G21" r:id="rId21" location="Nfi_lJ9ZpKk9RhLwSOvYd5mRaPkKkM4B-4cqv4ppf9U" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="G22" r:id="rId22" location="J7fEN89thcXGn94n15_wJl74cQGBn-RLoTnk3k_IA-M" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="G23" r:id="rId23" location="RZdhhHAXIkrJU1UReZqf2Eh1govJXu56xGzk0ykyTo0" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="G24" r:id="rId24" location="W7S5VFDoc2APi-3aQywqFBSyXAkUHKzWukN-60mtIks" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="G25" r:id="rId25" location="jIRKBORNkHhaBRHyCepl14wBYWbNUyitK7j2mLENKbc" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="G26" r:id="rId26" location="SfZujTtD9DXzAflWaw8q5a4mcrX8-k37lIrTECb1gNs" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="G27" r:id="rId27" location="X6KHI1GKOdaR5uSjSH6vUKkR4i0OP8ERWQqIaIf2U3Q" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="G28" r:id="rId28" location="IR0hxJeFqvw3fVWLPeL9PTPx_Sk3ZRxeP9Bf2Vsr8Mc" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="G29" r:id="rId29" location="XunseXF_808g4CzMs1Ad2pXfI7krE2q0sTy6EET0nRA" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="G30" r:id="rId30" location="rBDf6zRJ4qXP3i82sRKnLA6Hs9G_Gp9cDRIE7ZfkifA" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="F3:F30" r:id="rId31" display="https://drive.google.com/file/d/1POOBmBqGIMqNGuME0VsWmDRKv9yrRVez/view?usp=sharing" xr:uid="{AA325859-8F0C-4B80-B1EE-04D95CDCEDB4}"/>
+    <hyperlink ref="F30" r:id="rId32" xr:uid="{7D6AC8BE-2F4E-40B9-A7CF-25885EC48A40}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId59"/>
+    <tablePart r:id="rId33"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>